<commit_message>
Refactor&code for card view
</commit_message>
<xml_diff>
--- a/excel/T-通用配置.xlsx
+++ b/excel/T-通用配置.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCAA0FD-6843-4DE4-9CC0-6192EA81B987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F9C265-5A4A-406B-85D9-91A025F9C911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4620" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>导出类型</t>
   </si>
@@ -108,6 +108,14 @@
   </si>
   <si>
     <t>cardDisassembleReturnRatio</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大卡组数量</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>maxGroupNum</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1126,7 +1134,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1247,8 +1255,15 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="11">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>

</xml_diff>